<commit_message>
Signed-off-by: Jigar Mehta Global <jigar.digital@gmail.com>
</commit_message>
<xml_diff>
--- a/Git Tutorials Content.xlsx
+++ b/Git Tutorials Content.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="16215" windowHeight="9225" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="16215" windowHeight="9225" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="384">
   <si>
     <t>https://dzone.com/articles/version-control-git-vs-svn</t>
   </si>
@@ -486,9 +486,6 @@
     <t>Git Introduction &amp; Terminologies</t>
   </si>
   <si>
-    <t>Understand Git Folder Structure</t>
-  </si>
-  <si>
     <t>Configure Git</t>
   </si>
   <si>
@@ -562,9 +559,6 @@
   </si>
   <si>
     <t>How to configure username and gmail?</t>
-  </si>
-  <si>
-    <t>How to write our own 'git config' commands using 'git help'</t>
   </si>
   <si>
     <t>How to create local .git repository and check current status of repository?</t>
@@ -922,12 +916,6 @@
     <t>What is Tree, Commit and Branches?</t>
   </si>
   <si>
-    <t>Make PPT</t>
-  </si>
-  <si>
-    <t>Demo git init commands</t>
-  </si>
-  <si>
     <t>Demo Tree diagram</t>
   </si>
   <si>
@@ -1268,13 +1256,109 @@
   </si>
   <si>
     <t>Check System config file, output only the names of config variables for --list or --get-regexp</t>
+  </si>
+  <si>
+    <t>Understand Git Repository Layout</t>
+  </si>
+  <si>
+    <t>Demo git init commands
+Global Config path: 
+C:/Users/jigar.mehta1/.gitconfig
+System Config Path:
+C:/Program Files/Git/mingw64/etc/gitconfig</t>
+  </si>
+  <si>
+    <t>Global Config path: 
+C:/Users/jigar.mehta1/.gitconfig
+System Config Path:
+C:/Program Files/Git/mingw64/etc/gitconfig</t>
+  </si>
+  <si>
+    <t>Demo git status</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>git status</t>
+  </si>
+  <si>
+    <t>git status -s | git status --short</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Displays differences between the working tree and the staging area (will be shown in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>RED colour</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, between the staging area and the current HEAD commit (will be shows in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Green</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> colour.)</t>
+    </r>
+  </si>
+  <si>
+    <t>Show the output in the short-format. D for Deleted, M for Modified, ?? for newly added file. Unstaged files and folders will be in RED and Uncommited will be in Green</t>
+  </si>
+  <si>
+    <t>git status --porcelain</t>
+  </si>
+  <si>
+    <t>Shows all untracked and uncommited changes in short however with no colour differentiation</t>
+  </si>
+  <si>
+    <t>Give the output in the long-format. This is the default.</t>
+  </si>
+  <si>
+    <t>git status --long | git status</t>
+  </si>
+  <si>
+    <t>git status -v | git status --verbose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In addition to the names of files that have been changed, also show the textual changes that are staged to be committed </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1322,6 +1406,22 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2352,10 +2452,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:G73"/>
+  <dimension ref="A2:G72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2364,12 +2464,12 @@
     <col min="3" max="3" width="28" style="3" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="55.140625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="34.7109375" customWidth="1"/>
+    <col min="6" max="6" width="49.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B2" t="s">
         <v>116</v>
@@ -2390,7 +2490,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -2402,10 +2502,10 @@
         <v>1</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="F3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30">
@@ -2413,10 +2513,10 @@
         <v>2</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="F4" t="s">
         <v>207</v>
-      </c>
-      <c r="F4" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="30">
@@ -2424,26 +2524,26 @@
         <v>3</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F5" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="225">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="210">
       <c r="D6">
         <v>4</v>
       </c>
       <c r="E6" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="30">
+    </row>
+    <row r="7" spans="1:7" ht="75">
       <c r="A7" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -2455,10 +2555,10 @@
         <v>5</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>258</v>
+        <v>370</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30">
@@ -2466,10 +2566,10 @@
         <v>6</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F8" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -2477,10 +2577,10 @@
         <v>7</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F9" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -2488,27 +2588,30 @@
         <v>8</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>122</v>
+        <v>369</v>
       </c>
       <c r="F10" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="60">
       <c r="A11" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B11">
         <v>3</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D11">
         <v>9</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>261</v>
+        <v>257</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -2516,7 +2619,10 @@
         <v>10</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
+      </c>
+      <c r="F12" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="30">
@@ -2524,10 +2630,10 @@
         <v>11</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -2535,43 +2641,46 @@
         <v>12</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F14" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="30">
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="15" spans="1:7">
       <c r="D15">
         <v>13</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
+      </c>
+      <c r="F15" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="30">
-      <c r="B16">
-        <v>4</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>127</v>
-      </c>
       <c r="D16">
         <v>14</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" ht="30">
+        <v>132</v>
+      </c>
+      <c r="F16" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7">
       <c r="D17">
         <v>15</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>133</v>
-      </c>
-      <c r="F17" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="18" spans="2:7">
@@ -2579,7 +2688,10 @@
         <v>16</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>134</v>
+        <v>129</v>
+      </c>
+      <c r="F18" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="19" spans="2:7">
@@ -2587,10 +2699,13 @@
         <v>17</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F19" t="s">
-        <v>139</v>
+        <v>127</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="2:7">
@@ -2598,13 +2713,10 @@
         <v>18</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F20" t="s">
         <v>128</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="21" spans="2:7">
@@ -2612,10 +2724,7 @@
         <v>19</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F21" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
     </row>
     <row r="22" spans="2:7">
@@ -2623,7 +2732,10 @@
         <v>20</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>135</v>
+        <v>173</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="23" spans="2:7">
@@ -2633,61 +2745,61 @@
       <c r="E23" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7">
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="2:7" ht="30">
+      <c r="B24">
+        <v>5</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>136</v>
+      </c>
       <c r="D24">
         <v>22</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="F24" s="1"/>
-    </row>
-    <row r="25" spans="2:7" ht="30">
-      <c r="B25">
-        <v>5</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>137</v>
-      </c>
+        <v>253</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7">
       <c r="D25">
         <v>23</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" ht="30">
       <c r="D26">
         <v>24</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" ht="30">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7">
+      <c r="B27">
+        <v>6</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="D27">
         <v>25</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
     </row>
     <row r="28" spans="2:7">
-      <c r="B28">
-        <v>6</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>79</v>
-      </c>
       <c r="D28">
         <v>26</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>136</v>
+        <v>155</v>
+      </c>
+      <c r="F28" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="29" spans="2:7">
@@ -2695,10 +2807,10 @@
         <v>27</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F29" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="30" spans="2:7">
@@ -2706,32 +2818,29 @@
         <v>28</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F30" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="31" spans="2:7">
+    <row r="31" spans="2:7" ht="30">
       <c r="D31">
         <v>29</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F31" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7" ht="30">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7">
       <c r="D32">
         <v>30</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="F32" t="s">
-        <v>142</v>
+        <v>158</v>
       </c>
     </row>
     <row r="33" spans="2:6">
@@ -2739,35 +2848,35 @@
         <v>31</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
+      </c>
+      <c r="F33" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="34" spans="2:6">
+      <c r="B34">
+        <v>7</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="D34">
         <v>32</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>161</v>
+        <v>145</v>
       </c>
       <c r="F34" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
     </row>
     <row r="35" spans="2:6">
-      <c r="B35">
-        <v>7</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>81</v>
-      </c>
       <c r="D35">
         <v>33</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="F35" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="36" spans="2:6">
@@ -2775,6 +2884,9 @@
         <v>34</v>
       </c>
       <c r="E36" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="F36" t="s">
         <v>152</v>
       </c>
     </row>
@@ -2785,16 +2897,13 @@
       <c r="E37" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="F37" t="s">
-        <v>154</v>
-      </c>
     </row>
     <row r="38" spans="2:6">
       <c r="D38">
         <v>36</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="39" spans="2:6">
@@ -2802,7 +2911,10 @@
         <v>37</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>156</v>
+        <v>161</v>
+      </c>
+      <c r="F39" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="40" spans="2:6">
@@ -2810,10 +2922,10 @@
         <v>38</v>
       </c>
       <c r="E40" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="F40" t="s">
         <v>163</v>
-      </c>
-      <c r="F40" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="41" spans="2:6">
@@ -2821,40 +2933,37 @@
         <v>39</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="F41" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="42" spans="2:6">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" ht="30">
       <c r="D42">
         <v>40</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="43" spans="2:6" ht="30">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6">
+      <c r="B43">
+        <v>8</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>83</v>
+      </c>
       <c r="D43">
         <v>41</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>181</v>
+        <v>164</v>
       </c>
     </row>
     <row r="44" spans="2:6">
-      <c r="B44">
-        <v>8</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>83</v>
-      </c>
       <c r="D44">
         <v>42</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="45" spans="2:6">
@@ -2862,7 +2971,7 @@
         <v>43</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="46" spans="2:6">
@@ -2870,7 +2979,7 @@
         <v>44</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="47" spans="2:6">
@@ -2878,7 +2987,7 @@
         <v>45</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="48" spans="2:6">
@@ -2886,73 +2995,73 @@
         <v>46</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="49" spans="2:6">
+      <c r="B49">
+        <v>9</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>176</v>
+      </c>
       <c r="D49">
         <v>47</v>
       </c>
       <c r="E49" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="F49" s="1" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="50" spans="2:6">
-      <c r="B50">
-        <v>9</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>178</v>
-      </c>
       <c r="D50">
         <v>48</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="F50" s="1" t="s">
-        <v>173</v>
-      </c>
+      <c r="F50" s="1"/>
     </row>
     <row r="51" spans="2:6">
       <c r="D51">
         <v>49</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="F51" s="1"/>
+        <v>177</v>
+      </c>
     </row>
     <row r="52" spans="2:6">
       <c r="D52">
         <v>50</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="53" spans="2:6">
+      <c r="B53">
+        <v>10</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>202</v>
+      </c>
       <c r="D53">
         <v>51</v>
       </c>
-      <c r="E53" s="3" t="s">
+      <c r="E53" t="s">
         <v>182</v>
       </c>
+      <c r="F53" s="1" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="54" spans="2:6">
-      <c r="B54">
-        <v>10</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>204</v>
-      </c>
       <c r="D54">
         <v>52</v>
       </c>
       <c r="E54" t="s">
-        <v>184</v>
-      </c>
-      <c r="F54" s="1" t="s">
         <v>183</v>
       </c>
     </row>
@@ -2961,7 +3070,7 @@
         <v>53</v>
       </c>
       <c r="E55" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="56" spans="2:6">
@@ -2969,7 +3078,7 @@
         <v>54</v>
       </c>
       <c r="E56" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="57" spans="2:6">
@@ -2977,7 +3086,7 @@
         <v>55</v>
       </c>
       <c r="E57" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="58" spans="2:6">
@@ -2985,7 +3094,7 @@
         <v>56</v>
       </c>
       <c r="E58" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="59" spans="2:6">
@@ -2993,7 +3102,7 @@
         <v>57</v>
       </c>
       <c r="E59" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="60" spans="2:6">
@@ -3001,7 +3110,7 @@
         <v>58</v>
       </c>
       <c r="E60" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="61" spans="2:6">
@@ -3009,7 +3118,7 @@
         <v>59</v>
       </c>
       <c r="E61" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="62" spans="2:6">
@@ -3017,7 +3126,7 @@
         <v>60</v>
       </c>
       <c r="E62" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="63" spans="2:6">
@@ -3025,7 +3134,7 @@
         <v>61</v>
       </c>
       <c r="E63" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="64" spans="2:6">
@@ -3033,7 +3142,7 @@
         <v>62</v>
       </c>
       <c r="E64" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="65" spans="4:5">
@@ -3041,7 +3150,7 @@
         <v>63</v>
       </c>
       <c r="E65" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="66" spans="4:5">
@@ -3049,7 +3158,7 @@
         <v>64</v>
       </c>
       <c r="E66" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="67" spans="4:5">
@@ -3057,7 +3166,7 @@
         <v>65</v>
       </c>
       <c r="E67" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="68" spans="4:5">
@@ -3065,7 +3174,7 @@
         <v>66</v>
       </c>
       <c r="E68" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="69" spans="4:5">
@@ -3073,7 +3182,7 @@
         <v>67</v>
       </c>
       <c r="E69" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="70" spans="4:5">
@@ -3081,7 +3190,7 @@
         <v>68</v>
       </c>
       <c r="E70" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="71" spans="4:5">
@@ -3089,7 +3198,7 @@
         <v>69</v>
       </c>
       <c r="E71" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="72" spans="4:5">
@@ -3097,24 +3206,16 @@
         <v>70</v>
       </c>
       <c r="E72" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="73" spans="4:5">
-      <c r="D73">
-        <v>71</v>
-      </c>
-      <c r="E73" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F14" r:id="rId1" location="EXAMPLES"/>
-    <hyperlink ref="G20" r:id="rId2" location="analyzechanges_in_githistory"/>
-    <hyperlink ref="F50" r:id="rId3" location="using-the-git-blame-command"/>
-    <hyperlink ref="F23" r:id="rId4" location="gitclean"/>
-    <hyperlink ref="F54" r:id="rId5"/>
+    <hyperlink ref="G19" r:id="rId2" location="analyzechanges_in_githistory"/>
+    <hyperlink ref="F49" r:id="rId3" location="using-the-git-blame-command"/>
+    <hyperlink ref="F22" r:id="rId4" location="gitclean"/>
+    <hyperlink ref="F53" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>
@@ -3139,72 +3240,72 @@
   <sheetData>
     <row r="2" spans="1:9">
       <c r="A2" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30">
       <c r="A5" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="75">
       <c r="A6" s="4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="30">
       <c r="A7" s="4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="E14" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -3405,10 +3506,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D66"/>
+  <dimension ref="A1:D71"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="41.42578125" defaultRowHeight="15"/>
@@ -3421,686 +3523,774 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>230</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="45">
       <c r="A2" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>235</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="75">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="60">
       <c r="A3" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="60">
       <c r="A5" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30">
       <c r="A7" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30">
       <c r="A8" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="120">
       <c r="A11" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="30">
       <c r="A12" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>262</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>271</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="30">
-      <c r="A17" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="30">
       <c r="A27" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="30">
       <c r="A28" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="30">
       <c r="A29" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="30">
       <c r="A40" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="30">
       <c r="A41" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="30">
       <c r="A42" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="30">
       <c r="A46" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="30">
       <c r="A47" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="30">
       <c r="A48" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="30">
       <c r="A49" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="30">
       <c r="A50" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="30">
       <c r="A51" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="C51" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
-      <c r="B52" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="C52" s="2" t="s">
+    <row r="54" spans="1:3">
+      <c r="A54" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
-      <c r="B53" s="2" t="s">
+    <row r="55" spans="1:3">
+      <c r="A55" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B55" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C55" s="2" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="B54" s="2" t="s">
-        <v>346</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
-      <c r="B55" s="2" t="s">
-        <v>349</v>
-      </c>
-      <c r="C55" s="2" t="s">
+      <c r="C57" s="2" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B59" s="2" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="56" spans="1:3">
-      <c r="B56" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="C56" s="2" t="s">
+      <c r="C59" s="2" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B60" s="2" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="B57" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
-      <c r="B58" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="C58" s="2" t="s">
+      <c r="C60" s="2" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="C61" s="2" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
-      <c r="B59" s="2" t="s">
-        <v>356</v>
-      </c>
-      <c r="C59" s="2" t="s">
+    <row r="62" spans="1:3">
+      <c r="A62" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B62" s="2" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="60" spans="1:3">
-      <c r="B60" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="C60" s="2" t="s">
+      <c r="C62" s="2" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B63" s="2" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="B61" s="2" t="s">
-        <v>361</v>
-      </c>
-      <c r="C61" s="2" t="s">
+      <c r="C63" s="2" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
-      <c r="B62" s="2" t="s">
+    <row r="64" spans="1:3">
+      <c r="A64" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B64" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="C64" s="2" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B66" s="2" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="63" spans="1:3">
-      <c r="B63" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3">
-      <c r="B64" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="65" spans="2:3">
-      <c r="B65" s="2" t="s">
+      <c r="C66" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="C65" s="2" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="66" spans="2:3">
-      <c r="B66" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>372</v>
+    </row>
+    <row r="67" spans="1:3" ht="30">
+      <c r="A67" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="30">
+      <c r="B68" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="B69" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="B70" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="B71" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>383</v>
       </c>
     </row>
   </sheetData>

</xml_diff>